<commit_message>
[Update] Behavior Desiner로 간단한 몬스터 추적AI 작성, Navmesh AI 패키지 추가
</commit_message>
<xml_diff>
--- a/Assets/Resource/Xlsx/GameData.xlsx
+++ b/Assets/Resource/Xlsx/GameData.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\UnityProject\ProjectCR\Assets\Resource\Xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\KGA\Documents\GitHub\ProjectCR\Assets\Resource\Xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{254DBF26-CB13-40A3-B588-BFF99482DAF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="2715" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="345" yWindow="2715" windowWidth="21600" windowHeight="11295" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LevelData" sheetId="4" r:id="rId1"/>
@@ -33,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="135">
   <si>
     <t>level</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -543,13 +542,33 @@
   </si>
   <si>
     <t>Test</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Passive</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Debuff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Hp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Mp</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AutoTargeting</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -886,7 +905,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1604,11 +1623,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1696,7 +1715,7 @@
         <v>124</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="K2">
         <v>10</v>
@@ -1711,7 +1730,7 @@
         <v>127</v>
       </c>
       <c r="O2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -1740,7 +1759,7 @@
         <v>2</v>
       </c>
       <c r="K3">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L3">
         <v>10</v>
@@ -1760,7 +1779,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E4" t="s">
         <v>129</v>
@@ -1772,16 +1791,16 @@
         <v>122</v>
       </c>
       <c r="H4" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="I4" t="s">
-        <v>124</v>
+        <v>132</v>
       </c>
       <c r="J4">
         <v>3</v>
       </c>
       <c r="K4">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="L4">
         <v>10</v>
@@ -1793,7 +1812,7 @@
         <v>127</v>
       </c>
       <c r="O4">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -1801,7 +1820,7 @@
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E5" t="s">
         <v>129</v>
@@ -1813,16 +1832,16 @@
         <v>122</v>
       </c>
       <c r="H5" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="I5" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
       <c r="J5">
         <v>4</v>
       </c>
       <c r="K5">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L5">
         <v>10</v>
@@ -1831,10 +1850,10 @@
         <v>125</v>
       </c>
       <c r="N5" t="s">
-        <v>127</v>
+        <v>134</v>
       </c>
       <c r="O5">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -1842,7 +1861,7 @@
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E6" t="s">
         <v>129</v>
@@ -1854,7 +1873,7 @@
         <v>122</v>
       </c>
       <c r="H6" t="s">
-        <v>123</v>
+        <v>131</v>
       </c>
       <c r="I6" t="s">
         <v>124</v>
@@ -1863,7 +1882,7 @@
         <v>5</v>
       </c>
       <c r="K6">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="L6">
         <v>10</v>
@@ -1875,7 +1894,7 @@
         <v>127</v>
       </c>
       <c r="O6">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -1889,7 +1908,7 @@
         <v>123</v>
       </c>
       <c r="D7" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E7" t="s">
         <v>129</v>
@@ -1922,7 +1941,7 @@
         <v>127</v>
       </c>
       <c r="O7">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -1930,7 +1949,7 @@
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="E8" t="s">
         <v>129</v>
@@ -1963,7 +1982,7 @@
         <v>127</v>
       </c>
       <c r="O8">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -1982,7 +2001,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2055,7 +2074,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2185,7 +2204,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2233,7 +2252,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2282,7 +2301,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -2330,7 +2349,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2521,7 +2540,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>